<commit_message>
Updated the path of data and updated gene names venn
</commit_message>
<xml_diff>
--- a/data/Venn_Diagrams/Gene_name_data/GENES_All_GENES_VENN_DATA.xlsx
+++ b/data/Venn_Diagrams/Gene_name_data/GENES_All_GENES_VENN_DATA.xlsx
@@ -434,26 +434,40 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>6</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>DESeq2/LimmaVoom/EdgeR</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>DESeq2/EdgeR</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DESeq2/LimmaVoom</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>EdgeR/LimmaVoom</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>DESeq2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>LimmaVoom</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>EdgeR</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -464,7 +478,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RPS9</t>
+          <t>CROCCP2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -497,7 +511,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CROCCP2</t>
+          <t>RPS9</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1116,7 +1130,7 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ZNF462</t>
+          <t>RP11-420C9.1</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1145,7 +1159,7 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>RP11-420C9.1</t>
+          <t>ZNF462</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1242,7 +1256,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>NME2P1</t>
+          <t>CH507-528H12.1</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1285,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>PDE3A</t>
+          <t>NME2P1</t>
         </is>
       </c>
     </row>
@@ -1300,7 +1314,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>CH507-528H12.1</t>
+          <t>PDE3A</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1454,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>SOCS1</t>
+          <t>AC016757.3</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1469,7 +1483,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>AC016757.3</t>
+          <t>SOCS1</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1585,7 +1599,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>NEO1</t>
+          <t>CTD-2007H13.3</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1614,7 +1628,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>CTD-2007H13.3</t>
+          <t>NEO1</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1701,7 +1715,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Y_RNA</t>
+          <t>CTD-2186M15.3</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -1730,7 +1744,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>ZNF252P-AS1</t>
+          <t>Y_RNA</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -1759,7 +1773,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>CTD-2186M15.3</t>
+          <t>ZNF252P-AS1</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -1996,7 +2010,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>RP11-545I5.3</t>
+          <t>RP11-531H8.2</t>
         </is>
       </c>
     </row>
@@ -2025,7 +2039,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>RP11-531H8.2</t>
+          <t>RP11-545I5.3</t>
         </is>
       </c>
     </row>

</xml_diff>